<commit_message>
Dev tính năng LCD
</commit_message>
<xml_diff>
--- a/DiemDanh.xlsx
+++ b/DiemDanh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkingZone\FGA-Traing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A2972D-B78E-4A32-9E1B-A83F83955A49}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8AB492-7AA9-43A6-8E74-8399F81BB572}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="-120" windowWidth="27930" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="107">
   <si>
     <t>Lã Tuấn Vinh</t>
   </si>
@@ -905,11 +905,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF31"/>
+  <dimension ref="A1:AH31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD31" sqref="AD31"/>
+      <pane xSplit="5" topLeftCell="AA1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AF5" sqref="AF5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +928,7 @@
     <col min="19" max="19" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -1007,8 +1007,16 @@
         <v>43656</v>
       </c>
       <c r="AD1" s="23"/>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE1" s="22">
+        <v>43657</v>
+      </c>
+      <c r="AF1" s="23"/>
+      <c r="AG1" s="22">
+        <v>43658</v>
+      </c>
+      <c r="AH1" s="23"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1072,8 +1080,12 @@
       <c r="AB2" s="19"/>
       <c r="AC2" s="19"/>
       <c r="AD2" s="19"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="19"/>
+      <c r="AG2" s="19"/>
+      <c r="AH2" s="19"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1125,8 +1137,12 @@
       <c r="AB3" s="19"/>
       <c r="AC3" s="19"/>
       <c r="AD3" s="19"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
+      <c r="AG3" s="19"/>
+      <c r="AH3" s="19"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1180,8 +1196,12 @@
       <c r="AB4" s="19"/>
       <c r="AC4" s="19"/>
       <c r="AD4" s="19"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE4" s="19"/>
+      <c r="AF4" s="19"/>
+      <c r="AG4" s="19"/>
+      <c r="AH4" s="19"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1232,8 +1252,12 @@
       <c r="AB5" s="19"/>
       <c r="AC5" s="19"/>
       <c r="AD5" s="19"/>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="19"/>
+      <c r="AG5" s="19"/>
+      <c r="AH5" s="19"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1291,8 +1315,12 @@
       </c>
       <c r="AC6" s="20"/>
       <c r="AD6" s="20"/>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="20"/>
+      <c r="AG6" s="20"/>
+      <c r="AH6" s="20"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -1350,8 +1378,14 @@
       <c r="AB7" s="20"/>
       <c r="AC7" s="20"/>
       <c r="AD7" s="20"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG7" s="20"/>
+      <c r="AH7" s="20"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -1410,8 +1444,12 @@
       <c r="AB8" s="20"/>
       <c r="AC8" s="20"/>
       <c r="AD8" s="20"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE8" s="20"/>
+      <c r="AF8" s="20"/>
+      <c r="AG8" s="20"/>
+      <c r="AH8" s="20"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -1469,8 +1507,14 @@
       <c r="AB9" s="20"/>
       <c r="AC9" s="20"/>
       <c r="AD9" s="20"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG9" s="20"/>
+      <c r="AH9" s="20"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1536,8 +1580,12 @@
       <c r="AB10" s="19"/>
       <c r="AC10" s="19"/>
       <c r="AD10" s="19"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE10" s="19"/>
+      <c r="AF10" s="19"/>
+      <c r="AG10" s="19"/>
+      <c r="AH10" s="19"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1595,8 +1643,12 @@
       <c r="AB11" s="19"/>
       <c r="AC11" s="19"/>
       <c r="AD11" s="19"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE11" s="19"/>
+      <c r="AF11" s="19"/>
+      <c r="AG11" s="19"/>
+      <c r="AH11" s="19"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1647,8 +1699,12 @@
       <c r="AB12" s="19"/>
       <c r="AC12" s="19"/>
       <c r="AD12" s="19"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE12" s="19"/>
+      <c r="AF12" s="19"/>
+      <c r="AG12" s="19"/>
+      <c r="AH12" s="19"/>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -1699,8 +1755,12 @@
       <c r="AB13" s="19"/>
       <c r="AC13" s="19"/>
       <c r="AD13" s="19"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE13" s="19"/>
+      <c r="AF13" s="19"/>
+      <c r="AG13" s="19"/>
+      <c r="AH13" s="19"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -1759,8 +1819,12 @@
       <c r="AB14" s="19"/>
       <c r="AC14" s="19"/>
       <c r="AD14" s="19"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE14" s="19"/>
+      <c r="AF14" s="19"/>
+      <c r="AG14" s="19"/>
+      <c r="AH14" s="19"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -1818,8 +1882,12 @@
       <c r="AB15" s="20"/>
       <c r="AC15" s="20"/>
       <c r="AD15" s="20"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE15" s="20"/>
+      <c r="AF15" s="20"/>
+      <c r="AG15" s="20"/>
+      <c r="AH15" s="20"/>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>15</v>
       </c>
@@ -1885,8 +1953,12 @@
       <c r="AB16" s="20"/>
       <c r="AC16" s="20"/>
       <c r="AD16" s="20"/>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE16" s="20"/>
+      <c r="AF16" s="20"/>
+      <c r="AG16" s="20"/>
+      <c r="AH16" s="20"/>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -1942,8 +2014,12 @@
       <c r="AB17" s="20"/>
       <c r="AC17" s="20"/>
       <c r="AD17" s="20"/>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE17" s="20"/>
+      <c r="AF17" s="20"/>
+      <c r="AG17" s="20"/>
+      <c r="AH17" s="20"/>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -2004,8 +2080,12 @@
       <c r="AB18" s="20"/>
       <c r="AC18" s="20"/>
       <c r="AD18" s="20"/>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE18" s="20"/>
+      <c r="AF18" s="20"/>
+      <c r="AG18" s="20"/>
+      <c r="AH18" s="20"/>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -2059,8 +2139,12 @@
       <c r="AB19" s="19"/>
       <c r="AC19" s="19"/>
       <c r="AD19" s="19"/>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE19" s="19"/>
+      <c r="AF19" s="19"/>
+      <c r="AG19" s="19"/>
+      <c r="AH19" s="19"/>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -2103,8 +2187,12 @@
       <c r="AB20" s="19"/>
       <c r="AC20" s="19"/>
       <c r="AD20" s="19"/>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE20" s="19"/>
+      <c r="AF20" s="19"/>
+      <c r="AG20" s="19"/>
+      <c r="AH20" s="19"/>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -2164,8 +2252,12 @@
       <c r="AB21" s="19"/>
       <c r="AC21" s="19"/>
       <c r="AD21" s="19"/>
-    </row>
-    <row r="22" spans="1:32" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE21" s="19"/>
+      <c r="AF21" s="19"/>
+      <c r="AG21" s="19"/>
+      <c r="AH21" s="19"/>
+    </row>
+    <row r="22" spans="1:34" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -2218,10 +2310,14 @@
       <c r="AB22" s="19"/>
       <c r="AC22" s="19"/>
       <c r="AD22" s="19"/>
-      <c r="AE22"/>
-      <c r="AF22"/>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE22" s="19"/>
+      <c r="AF22" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG22" s="19"/>
+      <c r="AH22" s="19"/>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>22</v>
       </c>
@@ -2274,8 +2370,12 @@
       <c r="AB23" s="20"/>
       <c r="AC23" s="20"/>
       <c r="AD23" s="20"/>
-    </row>
-    <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE23" s="20"/>
+      <c r="AF23" s="20"/>
+      <c r="AG23" s="20"/>
+      <c r="AH23" s="20"/>
+    </row>
+    <row r="24" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>23</v>
       </c>
@@ -2328,8 +2428,16 @@
       <c r="AB24" s="20"/>
       <c r="AC24" s="20"/>
       <c r="AD24" s="20"/>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE24" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF24" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG24" s="20"/>
+      <c r="AH24" s="20"/>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>24</v>
       </c>
@@ -2378,8 +2486,12 @@
       <c r="AB25" s="20"/>
       <c r="AC25" s="20"/>
       <c r="AD25" s="20"/>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE25" s="20"/>
+      <c r="AF25" s="20"/>
+      <c r="AG25" s="20"/>
+      <c r="AH25" s="20"/>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>25</v>
       </c>
@@ -2433,8 +2545,12 @@
       <c r="AB26" s="20"/>
       <c r="AC26" s="20"/>
       <c r="AD26" s="20"/>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE26" s="20"/>
+      <c r="AF26" s="20"/>
+      <c r="AG26" s="20"/>
+      <c r="AH26" s="20"/>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>26</v>
       </c>
@@ -2489,8 +2605,12 @@
       <c r="AB27" s="20"/>
       <c r="AC27" s="20"/>
       <c r="AD27" s="20"/>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE27" s="20"/>
+      <c r="AF27" s="20"/>
+      <c r="AG27" s="20"/>
+      <c r="AH27" s="20"/>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -2548,8 +2668,12 @@
       <c r="AB28" s="19"/>
       <c r="AC28" s="19"/>
       <c r="AD28" s="19"/>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE28" s="19"/>
+      <c r="AF28" s="19"/>
+      <c r="AG28" s="19"/>
+      <c r="AH28" s="19"/>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -2606,8 +2730,12 @@
       <c r="AB29" s="19"/>
       <c r="AC29" s="19"/>
       <c r="AD29" s="19"/>
-    </row>
-    <row r="30" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE29" s="19"/>
+      <c r="AF29" s="19"/>
+      <c r="AG29" s="19"/>
+      <c r="AH29" s="19"/>
+    </row>
+    <row r="30" spans="1:34" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -2664,10 +2792,12 @@
       <c r="AB30" s="19"/>
       <c r="AC30" s="19"/>
       <c r="AD30" s="19"/>
-      <c r="AE30"/>
-      <c r="AF30"/>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AE30" s="19"/>
+      <c r="AF30" s="19"/>
+      <c r="AG30" s="19"/>
+      <c r="AH30" s="19"/>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -2724,10 +2854,16 @@
       <c r="AB31" s="19"/>
       <c r="AC31" s="19"/>
       <c r="AD31" s="19"/>
+      <c r="AE31" s="19"/>
+      <c r="AF31" s="19"/>
+      <c r="AG31" s="19"/>
+      <c r="AH31" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E20" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="13">
+  <mergeCells count="15">
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AC1:AD1"/>
     <mergeCell ref="K23:K27"/>
     <mergeCell ref="K28:K31"/>

</xml_diff>